<commit_message>
add fig_main - update second report
</commit_message>
<xml_diff>
--- a/Data_IDB/corregido.xlsx
+++ b/Data_IDB/corregido.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="148">
   <si>
     <t>corregido</t>
   </si>
@@ -461,6 +461,9 @@
   </si>
   <si>
     <t>ok, se intersecta con el cultivo de aguacate</t>
+  </si>
+  <si>
+    <t>patca</t>
   </si>
 </sst>
 </file>
@@ -950,7 +953,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -958,6 +961,9 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -4058,10 +4064,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H10"/>
+  <dimension ref="B2:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4072,7 +4078,7 @@
     <col min="6" max="6" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -4082,8 +4088,17 @@
       <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="J2" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -4093,8 +4108,17 @@
       <c r="D3" s="2">
         <v>22.99</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="J3" s="4">
+        <v>0</v>
+      </c>
+      <c r="K3" s="4">
+        <v>248</v>
+      </c>
+      <c r="L3" s="4">
+        <v>65.782493000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>141</v>
       </c>
@@ -4113,8 +4137,17 @@
       <c r="H4">
         <v>17.93</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="J4" s="4">
+        <v>1</v>
+      </c>
+      <c r="K4" s="4">
+        <v>129</v>
+      </c>
+      <c r="L4" s="4">
+        <v>34.217506999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>143</v>
       </c>
@@ -4134,7 +4167,7 @@
         <v>5.98</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>142</v>
       </c>
@@ -4145,13 +4178,13 @@
         <v>10.34</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C7">
         <f>SUM(C3:C6)</f>
         <v>522</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="G8">
         <v>435</v>
       </c>
@@ -4159,20 +4192,20 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F9">
         <f>+C4-G4</f>
         <v>200</v>
       </c>
       <c r="G9">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="H9">
         <f>+G9*H8</f>
-        <v>5300</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C10">
         <f>SUM(C3:C9)</f>
         <v>1044</v>
@@ -4183,7 +4216,7 @@
       </c>
       <c r="H10" s="1">
         <f>+H9/G8</f>
-        <v>12.183908045977011</v>
+        <v>13.333333333333334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>